<commit_message>
Se actualiza automáticamente también precio total
</commit_message>
<xml_diff>
--- a/Auto-Excel/InventarioV2.xlsx
+++ b/Auto-Excel/InventarioV2.xlsx
@@ -524,7 +524,7 @@
         <v>5.25</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>50</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="3">
@@ -548,7 +548,7 @@
         <v>3.15</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
@@ -572,7 +572,7 @@
         <v>4.2</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
@@ -596,7 +596,7 @@
         <v>2.1</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
@@ -620,7 +620,7 @@
         <v>1.05</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>25</v>
+        <v>26.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>